<commit_message>
Added files for Photo and Test Report Test Cases
</commit_message>
<xml_diff>
--- a/src/main/resources/testdata.xlsx
+++ b/src/main/resources/testdata.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView windowWidth="28000" windowHeight="11520" tabRatio="500" firstSheet="8" activeTab="11"/>
+    <workbookView windowWidth="28000" windowHeight="11520" tabRatio="500" firstSheet="9" activeTab="12"/>
   </bookViews>
   <sheets>
     <sheet name="GeneralConfig" sheetId="1" r:id="rId1"/>
@@ -20,13 +20,14 @@
     <sheet name="VitalSignsTest" sheetId="10" r:id="rId10"/>
     <sheet name="NoteTest" sheetId="11" r:id="rId11"/>
     <sheet name="PhotoTest" sheetId="12" r:id="rId12"/>
+    <sheet name="TestReportTest" sheetId="13" r:id="rId13"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96">
   <si>
     <t>Parameters</t>
   </si>
@@ -295,7 +296,25 @@
     <t>choosefavoritephoto</t>
   </si>
   <si>
+    <t>negativescenerios</t>
+  </si>
+  <si>
+    <t>uploadtestreport</t>
+  </si>
+  <si>
+    <t>Automation_Test,Vibhor,model,Test.jpeg,Test Description</t>
+  </si>
+  <si>
+    <t>uploadtestreportwithotheroption</t>
+  </si>
+  <si>
+    <t>updatetestreport</t>
+  </si>
+  <si>
     <t>run</t>
+  </si>
+  <si>
+    <t>Automation_Test,Vibhor,model,Updated Description,Test Description</t>
   </si>
 </sst>
 </file>
@@ -304,9 +323,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
   </numFmts>
   <fonts count="28">
     <font>
@@ -366,6 +385,82 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -379,33 +474,11 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -418,15 +491,22 @@
     </font>
     <font>
       <b/>
-      <sz val="15"/>
-      <color theme="3"/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -445,67 +525,6 @@
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -516,25 +535,175 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -546,157 +715,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -707,6 +726,24 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -725,10 +762,42 @@
       <diagonal/>
     </border>
     <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="medium">
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
         <color theme="4"/>
       </bottom>
       <diagonal/>
@@ -757,189 +826,139 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="7" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="8" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="4" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="8" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="8" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="7" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="17" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="8" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="7" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="41" fontId="8" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="42" fontId="8" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="8" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="18" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="9" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="8" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -947,7 +966,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -957,9 +976,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="48" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
@@ -1311,7 +1327,7 @@
   <dimension ref="A1:B19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1015625" defaultRowHeight="14" outlineLevelCol="1"/>
@@ -1323,147 +1339,147 @@
   </cols>
   <sheetData>
     <row r="1" ht="22" spans="1:2">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="11" t="s">
+      <c r="B1" s="10" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" ht="22" spans="1:2">
-      <c r="A2" s="11" t="s">
+      <c r="A2" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="5" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="3" ht="22" spans="1:2">
-      <c r="A3" s="11" t="s">
+      <c r="A3" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="5" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="4" ht="22" spans="1:2">
-      <c r="A4" s="11" t="s">
+      <c r="A4" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="12" t="s">
+      <c r="B4" s="11" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="5" ht="22" spans="1:2">
-      <c r="A5" s="11" t="s">
+      <c r="A5" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="B5" s="5" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="6" ht="22" spans="1:2">
-      <c r="A6" s="11" t="s">
+      <c r="A6" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="B6" s="5" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="7" ht="22" spans="1:2">
-      <c r="A7" s="11" t="s">
+      <c r="A7" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="6">
+      <c r="B7" s="5">
         <v>4723</v>
       </c>
     </row>
     <row r="8" ht="22" spans="1:2">
-      <c r="A8" s="11" t="s">
+      <c r="A8" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="B8" s="6" t="s">
+      <c r="B8" s="5" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="9" ht="22" spans="1:2">
-      <c r="A9" s="11" t="s">
+      <c r="A9" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="B9" s="6">
+      <c r="B9" s="5">
         <v>13.3</v>
       </c>
     </row>
     <row r="10" ht="22" spans="1:2">
-      <c r="A10" s="11" t="s">
+      <c r="A10" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="B10" s="6"/>
+      <c r="B10" s="5"/>
     </row>
     <row r="11" ht="22" spans="1:2">
-      <c r="A11" s="11" t="s">
+      <c r="A11" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="B11" s="13"/>
+      <c r="B11" s="12"/>
     </row>
     <row r="12" ht="22" spans="1:2">
-      <c r="A12" s="11" t="s">
+      <c r="A12" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="B12" s="6"/>
+      <c r="B12" s="5"/>
     </row>
     <row r="13" ht="22" spans="1:2">
-      <c r="A13" s="11" t="s">
+      <c r="A13" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="B13" s="6" t="s">
+      <c r="B13" s="5" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="14" ht="22" spans="1:2">
-      <c r="A14" s="11" t="s">
+      <c r="A14" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="B14" s="6"/>
+      <c r="B14" s="5"/>
     </row>
     <row r="15" ht="22" spans="1:2">
-      <c r="A15" s="11" t="s">
+      <c r="A15" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="B15" s="14" t="b">
+      <c r="B15" s="13" t="b">
         <f>FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="16" ht="22" spans="1:2">
-      <c r="A16" s="11" t="s">
+      <c r="A16" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="B16" s="6" t="s">
+      <c r="B16" s="5" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="17" ht="22" spans="1:2">
-      <c r="A17" s="11" t="s">
+      <c r="A17" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="B17" s="6" t="s">
+      <c r="B17" s="5" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="18" ht="22" spans="1:2">
-      <c r="A18" s="11" t="s">
+      <c r="A18" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="B18" s="6" t="s">
+      <c r="B18" s="5" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="19" ht="22" spans="1:2">
-      <c r="A19" s="11" t="s">
+      <c r="A19" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="B19" s="6" t="s">
+      <c r="B19" s="5" t="s">
         <v>26</v>
       </c>
     </row>
@@ -1635,7 +1651,7 @@
       </c>
     </row>
     <row r="5" spans="1:3">
-      <c r="A5" s="5" t="s">
+      <c r="A5" s="4" t="s">
         <v>81</v>
       </c>
       <c r="B5" t="s">
@@ -1654,13 +1670,13 @@
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K25" sqref="K25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelRow="6" outlineLevelCol="2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelRow="7" outlineLevelCol="2"/>
   <cols>
     <col min="1" max="1" width="31.3828125" customWidth="1"/>
     <col min="2" max="2" width="19.53125" customWidth="1"/>
@@ -1708,7 +1724,7 @@
       </c>
     </row>
     <row r="5" spans="1:2">
-      <c r="A5" s="5" t="s">
+      <c r="A5" s="4" t="s">
         <v>86</v>
       </c>
       <c r="B5" t="s">
@@ -1728,10 +1744,86 @@
         <v>88</v>
       </c>
       <c r="B7" t="s">
-        <v>89</v>
+        <v>33</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>83</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" t="s">
+        <v>89</v>
+      </c>
+      <c r="B8" t="s">
+        <v>33</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>83</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr/>
+  <dimension ref="A1:C4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N24" sqref="N24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelRow="3" outlineLevelCol="2"/>
+  <cols>
+    <col min="1" max="1" width="29.171875" customWidth="1"/>
+    <col min="3" max="3" width="32.2890625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="22" spans="1:3">
+      <c r="A1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" t="s">
+        <v>92</v>
+      </c>
+      <c r="B3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" t="s">
+        <v>93</v>
+      </c>
+      <c r="B4" t="s">
+        <v>94</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>95</v>
       </c>
     </row>
   </sheetData>
@@ -1768,31 +1860,31 @@
       </c>
     </row>
     <row r="2" ht="22" spans="1:3">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="B2" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="C2" s="9"/>
+      <c r="B2" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C2" s="8"/>
     </row>
     <row r="3" ht="22" spans="1:3">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="B3" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="C3" s="9"/>
+      <c r="B3" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="C3" s="8"/>
     </row>
     <row r="4" ht="22" spans="1:3">
-      <c r="A4" s="6" t="s">
+      <c r="A4" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="B4" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="C4" s="9"/>
+      <c r="B4" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="C4" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.510416666666667" footer="0.510416666666667"/>
@@ -1829,13 +1921,13 @@
       </c>
     </row>
     <row r="2" ht="22" spans="1:3">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="B2" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="C2" s="7" t="s">
+      <c r="B2" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C2" s="6" t="s">
         <v>37</v>
       </c>
     </row>
@@ -1846,7 +1938,7 @@
       <c r="B3" t="s">
         <v>33</v>
       </c>
-      <c r="C3" s="8" t="s">
+      <c r="C3" s="7" t="s">
         <v>39</v>
       </c>
     </row>
@@ -1892,24 +1984,24 @@
       </c>
     </row>
     <row r="2" ht="22" spans="1:3">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="B2" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="C2" s="7" t="s">
+      <c r="B2" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C2" s="6" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="3" ht="22" spans="1:3">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="5" t="s">
         <v>42</v>
       </c>
       <c r="B3" t="s">
         <v>33</v>
       </c>
-      <c r="C3" s="8" t="s">
+      <c r="C3" s="7" t="s">
         <v>37</v>
       </c>
     </row>
@@ -1952,21 +2044,21 @@
       </c>
     </row>
     <row r="2" ht="22" spans="1:3">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="B2" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="C2" s="7" t="s">
+      <c r="B2" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C2" s="6" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="3" ht="22" spans="1:3">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="5" t="s">
         <v>33</v>
       </c>
       <c r="C3" t="s">
@@ -1977,7 +2069,7 @@
       <c r="A4" t="s">
         <v>47</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="5" t="s">
         <v>33</v>
       </c>
     </row>
@@ -1985,7 +2077,7 @@
       <c r="A5" t="s">
         <v>48</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="B5" s="5" t="s">
         <v>33</v>
       </c>
     </row>
@@ -1993,7 +2085,7 @@
       <c r="A6" t="s">
         <v>49</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="B6" s="5" t="s">
         <v>33</v>
       </c>
     </row>
@@ -2001,10 +2093,10 @@
       <c r="A7" t="s">
         <v>50</v>
       </c>
-      <c r="B7" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="C7" s="8" t="s">
+      <c r="B7" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C7" s="7" t="s">
         <v>51</v>
       </c>
     </row>
@@ -2047,13 +2139,13 @@
       </c>
     </row>
     <row r="2" ht="22" spans="1:3">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="5" t="s">
         <v>52</v>
       </c>
       <c r="B2" t="s">
         <v>33</v>
       </c>
-      <c r="C2" s="7"/>
+      <c r="C2" s="6"/>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
@@ -2097,13 +2189,13 @@
       </c>
     </row>
     <row r="2" ht="22" spans="1:3">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="B2" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="C2" s="7"/>
+      <c r="B2" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C2" s="6"/>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
@@ -2148,10 +2240,10 @@
       </c>
     </row>
     <row r="2" ht="22" spans="1:3">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="5" t="s">
         <v>33</v>
       </c>
       <c r="C2" s="3" t="s">
@@ -2226,10 +2318,10 @@
       </c>
     </row>
     <row r="2" ht="22" spans="1:3">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="5" t="s">
         <v>33</v>
       </c>
       <c r="C2" s="3" t="s">

</xml_diff>

<commit_message>
Added files relate to TestReport test case
</commit_message>
<xml_diff>
--- a/src/main/resources/testdata.xlsx
+++ b/src/main/resources/testdata.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97">
   <si>
     <t>Parameters</t>
   </si>
@@ -311,10 +311,13 @@
     <t>updatetestreport</t>
   </si>
   <si>
+    <t>Automation_Test,Vibhor,model,Updated Description,Test Description,vivek</t>
+  </si>
+  <si>
+    <t>negativescenerios_testreport</t>
+  </si>
+  <si>
     <t>run</t>
-  </si>
-  <si>
-    <t>Automation_Test,Vibhor,model,Updated Description,Test Description</t>
   </si>
 </sst>
 </file>
@@ -322,10 +325,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
   </numFmts>
   <fonts count="28">
     <font>
@@ -385,6 +388,104 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -398,6 +499,28 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF800080"/>
@@ -405,126 +528,6 @@
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -535,6 +538,180 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -542,180 +719,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -729,20 +732,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -762,17 +762,35 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
       </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
       </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
       </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -794,6 +812,15 @@
     <border>
       <left/>
       <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top style="thin">
         <color theme="4"/>
       </top>
@@ -802,163 +829,139 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="11" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="9" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="8" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="7" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="8" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="17" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="8" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="11" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="9" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="8" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="7" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="8" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="42" fontId="8" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="8" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="9" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="8" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1770,16 +1773,16 @@
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N24" sqref="N24"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelRow="3" outlineLevelCol="2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelRow="4" outlineLevelCol="2"/>
   <cols>
     <col min="1" max="1" width="29.171875" customWidth="1"/>
-    <col min="3" max="3" width="32.2890625" customWidth="1"/>
+    <col min="3" max="3" width="59.2421875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="22" spans="1:3">
@@ -1820,10 +1823,21 @@
         <v>93</v>
       </c>
       <c r="B4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C4" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="C4" s="3" t="s">
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" t="s">
         <v>95</v>
+      </c>
+      <c r="B5" t="s">
+        <v>96</v>
+      </c>
+      <c r="C5" t="s">
+        <v>91</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add Files related to Articles Test Case Automation
</commit_message>
<xml_diff>
--- a/src/main/resources/testdata.xlsx
+++ b/src/main/resources/testdata.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView windowWidth="28000" windowHeight="11520" tabRatio="500" firstSheet="9" activeTab="12"/>
+    <workbookView windowWidth="28000" windowHeight="11520" tabRatio="500" firstSheet="10" activeTab="13"/>
   </bookViews>
   <sheets>
     <sheet name="GeneralConfig" sheetId="1" r:id="rId1"/>
@@ -21,13 +21,14 @@
     <sheet name="NoteTest" sheetId="11" r:id="rId11"/>
     <sheet name="PhotoTest" sheetId="12" r:id="rId12"/>
     <sheet name="TestReportTest" sheetId="13" r:id="rId13"/>
+    <sheet name="ArticlesTest" sheetId="14" r:id="rId14"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102">
   <si>
     <t>Parameters</t>
   </si>
@@ -315,6 +316,21 @@
   </si>
   <si>
     <t>negativescenerios_testreport</t>
+  </si>
+  <si>
+    <t>addarticle</t>
+  </si>
+  <si>
+    <t>Yoga,The relaxation techniques,Steven</t>
+  </si>
+  <si>
+    <t>updatearticle</t>
+  </si>
+  <si>
+    <t>Yoga,The relaxation techniques,Steven,Updated Description</t>
+  </si>
+  <si>
+    <t>selectarticleasfavorite_unfavorite</t>
   </si>
   <si>
     <t>run</t>
@@ -326,9 +342,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
   </numFmts>
   <fonts count="28">
     <font>
@@ -384,6 +400,13 @@
       <sz val="10"/>
       <name val="Arial"/>
       <charset val="134"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
@@ -402,13 +425,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -423,13 +439,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="15"/>
       <color theme="3"/>
@@ -438,6 +447,44 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
@@ -446,28 +493,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color theme="3"/>
@@ -476,13 +501,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FF3F3F3F"/>
@@ -492,14 +510,6 @@
     </font>
     <font>
       <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -508,6 +518,20 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -515,17 +539,9 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color theme="1"/>
       <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -538,55 +554,169 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -598,127 +728,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -747,21 +763,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
@@ -781,16 +782,16 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF7F7F7F"/>
       </left>
       <right style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF7F7F7F"/>
       </right>
       <top style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF7F7F7F"/>
       </top>
       <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -812,15 +813,6 @@
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
       <top style="thin">
         <color theme="4"/>
       </top>
@@ -829,119 +821,143 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="9" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="7" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="8" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="11" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="9" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="30" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="17" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="7" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="41" fontId="8" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -951,17 +967,17 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="8" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="8" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1775,8 +1791,8 @@
   <sheetPr/>
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelRow="4" outlineLevelCol="2"/>
@@ -1834,10 +1850,76 @@
         <v>95</v>
       </c>
       <c r="B5" t="s">
-        <v>96</v>
+        <v>33</v>
       </c>
       <c r="C5" t="s">
         <v>91</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr/>
+  <dimension ref="A1:C4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelRow="3" outlineLevelCol="2"/>
+  <cols>
+    <col min="1" max="1" width="29.8203125" customWidth="1"/>
+    <col min="2" max="2" width="27.59375" customWidth="1"/>
+    <col min="3" max="3" width="64.84375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="22" spans="1:3">
+      <c r="A1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" t="s">
+        <v>98</v>
+      </c>
+      <c r="B3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" t="s">
+        <v>100</v>
+      </c>
+      <c r="B4" t="s">
+        <v>101</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>97</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added Music Test case related files
</commit_message>
<xml_diff>
--- a/src/main/resources/testdata.xlsx
+++ b/src/main/resources/testdata.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView windowWidth="28000" windowHeight="11520" tabRatio="500" firstSheet="10" activeTab="13"/>
+    <workbookView windowWidth="28000" windowHeight="11520" tabRatio="500" firstSheet="11" activeTab="14"/>
   </bookViews>
   <sheets>
     <sheet name="GeneralConfig" sheetId="1" r:id="rId1"/>
@@ -22,13 +22,14 @@
     <sheet name="PhotoTest" sheetId="12" r:id="rId12"/>
     <sheet name="TestReportTest" sheetId="13" r:id="rId13"/>
     <sheet name="ArticlesTest" sheetId="14" r:id="rId14"/>
+    <sheet name="MusicTest" sheetId="15" r:id="rId15"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106">
   <si>
     <t>Parameters</t>
   </si>
@@ -333,7 +334,19 @@
     <t>selectarticleasfavorite_unfavorite</t>
   </si>
   <si>
+    <t>addmusic</t>
+  </si>
+  <si>
+    <t>Test,Wait a minute it is coming right at us,Classical,Steven</t>
+  </si>
+  <si>
+    <t>updatemusic</t>
+  </si>
+  <si>
     <t>run</t>
+  </si>
+  <si>
+    <t>Test,Wait a minute it is coming right at us,Classical,Steven,Updated Title</t>
   </si>
 </sst>
 </file>
@@ -341,9 +354,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
   </numFmts>
   <fonts count="28">
@@ -397,11 +410,6 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <charset val="134"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color theme="0"/>
       <name val="Calibri"/>
@@ -411,6 +419,95 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -424,13 +521,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="18"/>
       <color theme="3"/>
@@ -439,47 +529,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -493,25 +544,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -523,27 +557,6 @@
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -560,181 +573,181 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -745,6 +758,80 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -766,82 +853,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
       <bottom style="double">
         <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -850,137 +863,137 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="7" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="8" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="30" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="17" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="7" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="8" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="10" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="7" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="11" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="11" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="7" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="11" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="11" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="8" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="8" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="8" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="11" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="17" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="11" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyBorder="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
@@ -1346,7 +1359,7 @@
   <dimension ref="A1:B19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1015625" defaultRowHeight="14" outlineLevelCol="1"/>
@@ -1867,8 +1880,8 @@
   <sheetPr/>
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1:C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelRow="3" outlineLevelCol="2"/>
@@ -1916,10 +1929,63 @@
         <v>100</v>
       </c>
       <c r="B4" t="s">
-        <v>101</v>
+        <v>33</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>97</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr/>
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I9" sqref="I9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelRow="2" outlineLevelCol="2"/>
+  <cols>
+    <col min="3" max="3" width="33.0703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="22" spans="1:3">
+      <c r="A1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" t="s">
+        <v>103</v>
+      </c>
+      <c r="B3" t="s">
+        <v>104</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>105</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added Camera and Movie Test Case Related Files
</commit_message>
<xml_diff>
--- a/src/main/resources/testdata.xlsx
+++ b/src/main/resources/testdata.xlsx
@@ -23,13 +23,14 @@
     <sheet name="TestReportTest" sheetId="13" r:id="rId13"/>
     <sheet name="ArticlesTest" sheetId="14" r:id="rId14"/>
     <sheet name="MusicTest" sheetId="15" r:id="rId15"/>
+    <sheet name="CameraTest" sheetId="16" r:id="rId16"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111">
   <si>
     <t>Parameters</t>
   </si>
@@ -337,19 +338,31 @@
     <t>addmusic</t>
   </si>
   <si>
-    <t>Test,Wait a minute it is coming right at us,Classical,Steven</t>
+    <t>Good Moon,Wait a minute it is coming right at us,Classical,Steven</t>
   </si>
   <si>
     <t>updatemusic</t>
   </si>
   <si>
-    <t>Test,Wait a minute it is coming right at us,Classical,Steven,Updated Title</t>
+    <t>Good Moon,Wait a minute it is coming right at us,Classical,Steven,Updated Title</t>
   </si>
   <si>
     <t>play_pause</t>
   </si>
   <si>
+    <t>selectmusicasfavorite_unfavorite</t>
+  </si>
+  <si>
+    <t>getinfo_download</t>
+  </si>
+  <si>
+    <t>picsave_crop</t>
+  </si>
+  <si>
     <t>run</t>
+  </si>
+  <si>
+    <t>picsave_full</t>
   </si>
 </sst>
 </file>
@@ -1950,14 +1963,15 @@
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelRow="3" outlineLevelCol="2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelRow="5" outlineLevelCol="2"/>
   <cols>
+    <col min="1" max="1" width="32.1640625" customWidth="1"/>
     <col min="3" max="3" width="33.0703125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1999,7 +2013,77 @@
         <v>105</v>
       </c>
       <c r="B4" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" t="s">
         <v>106</v>
+      </c>
+      <c r="B5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="B6" t="s">
+        <v>33</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>102</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr/>
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelRow="2" outlineLevelCol="2"/>
+  <cols>
+    <col min="1" max="1" width="20.3125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="22" spans="1:3">
+      <c r="A1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="C2" s="3"/>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="B3" t="s">
+        <v>109</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Code Refactoring for Batch Execution
</commit_message>
<xml_diff>
--- a/src/main/resources/testdata.xlsx
+++ b/src/main/resources/testdata.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView windowWidth="28000" windowHeight="11520" tabRatio="500" firstSheet="12" activeTab="13"/>
+    <workbookView windowWidth="28000" windowHeight="11520" tabRatio="500" firstSheet="9" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="GeneralConfig" sheetId="1" r:id="rId1"/>
@@ -263,6 +263,9 @@
     <t>addnote</t>
   </si>
   <si>
+    <t>run</t>
+  </si>
+  <si>
     <t>vibhor954,Test Description,Updated Description</t>
   </si>
   <si>
@@ -324,9 +327,6 @@
   </si>
   <si>
     <t>addarticle</t>
-  </si>
-  <si>
-    <t>run</t>
   </si>
   <si>
     <t>Yoga,The relaxation techniques,Steven</t>
@@ -374,8 +374,8 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="28">
@@ -436,6 +436,36 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -449,9 +479,23 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
-      <sz val="13"/>
+      <sz val="15"/>
       <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -465,6 +509,43 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
@@ -480,17 +561,11 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -501,81 +576,6 @@
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -586,103 +586,175 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -694,79 +766,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -790,21 +790,6 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
       <right style="thin">
@@ -819,28 +804,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -869,11 +837,43 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -882,134 +882,134 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="26" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="8" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="7" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="9" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="26" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="8" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="8" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="8" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="8" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="8" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="19" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="6" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="8" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="19" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="8" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="8" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="26" fillId="23" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="8" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1646,8 +1646,8 @@
   <sheetPr/>
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1:C5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelRow="4" outlineLevelCol="2"/>
@@ -1673,43 +1673,43 @@
         <v>76</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>33</v>
+        <v>77</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="C3" s="3" t="s">
         <v>78</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>79</v>
-      </c>
-      <c r="B4" t="s">
-        <v>33</v>
+        <v>80</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>77</v>
       </c>
       <c r="C4" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="C5" t="s">
         <v>81</v>
-      </c>
-      <c r="B5" t="s">
-        <v>33</v>
-      </c>
-      <c r="C5" t="s">
-        <v>80</v>
       </c>
     </row>
   </sheetData>
@@ -1724,7 +1724,7 @@
   <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K25" sqref="K25"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelRow="7" outlineLevelCol="2"/>
@@ -1746,70 +1746,70 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="2" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>33</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C3" s="3" t="s">
         <v>84</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>85</v>
-      </c>
-      <c r="B4" t="s">
+        <v>86</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="B5" t="s">
+        <v>87</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
-        <v>87</v>
-      </c>
-      <c r="B6" t="s">
+        <v>88</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" t="s">
-        <v>88</v>
-      </c>
-      <c r="B7" t="s">
+        <v>89</v>
+      </c>
+      <c r="B7" s="2" t="s">
         <v>33</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" t="s">
-        <v>89</v>
-      </c>
-      <c r="B8" t="s">
+        <v>90</v>
+      </c>
+      <c r="B8" s="2" t="s">
         <v>33</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
     </row>
   </sheetData>
@@ -1846,46 +1846,46 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="2" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>33</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="B3" t="s">
         <v>33</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="B4" t="s">
         <v>33</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="B5" t="s">
         <v>33</v>
       </c>
       <c r="C5" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
     </row>
   </sheetData>
@@ -1899,8 +1899,8 @@
   <sheetPr/>
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelRow="3" outlineLevelCol="2"/>
@@ -1923,10 +1923,10 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="2" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>98</v>
+        <v>33</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>99</v>
@@ -1937,7 +1937,7 @@
         <v>100</v>
       </c>
       <c r="B3" t="s">
-        <v>98</v>
+        <v>33</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>101</v>
@@ -2050,7 +2050,7 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelRow="2" outlineLevelCol="2"/>

</xml_diff>

<commit_message>
Fixed Email test cases issues
</commit_message>
<xml_diff>
--- a/src/main/resources/testdata.xlsx
+++ b/src/main/resources/testdata.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView windowWidth="28000" windowHeight="11520" tabRatio="500" firstSheet="13" activeTab="16"/>
+    <workbookView windowWidth="28000" windowHeight="12120" tabRatio="500" firstSheet="3" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="GeneralConfig" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114">
   <si>
     <t>Parameters</t>
   </si>
@@ -54,12 +54,15 @@
     <t>deviceNameAndroid</t>
   </si>
   <si>
-    <t>7ecac417</t>
+    <t>2YH3Y18831026822</t>
   </si>
   <si>
     <t>platformVersionAndroid</t>
   </si>
   <si>
+    <t>6.0.1</t>
+  </si>
+  <si>
     <t>appiumServerIp</t>
   </si>
   <si>
@@ -138,13 +141,13 @@
     <t>logout</t>
   </si>
   <si>
-    <t>loginwithvalidcredentials</t>
+    <t>t1_loginwithvalidcredentials</t>
   </si>
   <si>
     <t>vibhor954@gmail.com,Bsavib9!</t>
   </si>
   <si>
-    <t>loginwithinvalidcredentials</t>
+    <t>t2_loginwithinvalidcredentials</t>
   </si>
   <si>
     <t>test@test.com,test123,Enter your user id or email,vibhor954@gmail.com,Bsavib9!</t>
@@ -159,43 +162,46 @@
     <t>forgotpasswordwithvaliddata</t>
   </si>
   <si>
-    <t>sendemail</t>
+    <t>t1_sendemail</t>
+  </si>
+  <si>
+    <t>run</t>
   </si>
   <si>
     <t>vibhor954@gmail.com,Test Subject,Test Description,vibhor954</t>
   </si>
   <si>
-    <t>recieveemail</t>
+    <t>t2_recieveemail</t>
   </si>
   <si>
     <t>vibhor954</t>
   </si>
   <si>
-    <t>deleteemailsfrominbox</t>
-  </si>
-  <si>
-    <t>deleteemailsfromsent</t>
-  </si>
-  <si>
-    <t>deleteemailsfromtrash</t>
-  </si>
-  <si>
-    <t>emailnegativecases</t>
+    <t>t3_deleteemailsfrominbox</t>
+  </si>
+  <si>
+    <t>t4_deleteemailsfromsent</t>
+  </si>
+  <si>
+    <t>t5_deleteemailsfromtrash</t>
+  </si>
+  <si>
+    <t>t6_emailnegativecases</t>
   </si>
   <si>
     <t>vibhor954@gmail.com,Test Subject,Test Description</t>
   </si>
   <si>
-    <t>spritualitymeditation</t>
-  </si>
-  <si>
-    <t>spritualityvideos</t>
-  </si>
-  <si>
-    <t>verifyfacebook</t>
-  </si>
-  <si>
-    <t>verifytwitter</t>
+    <t>t1_spritualitymeditation</t>
+  </si>
+  <si>
+    <t>t2_spritualityvideos</t>
+  </si>
+  <si>
+    <t>t1_verifyfacebook</t>
+  </si>
+  <si>
+    <t>t2_verifytwitter</t>
   </si>
   <si>
     <t>verifysearch</t>
@@ -216,22 +222,22 @@
     <t>makedoctorappointment_doctornotavailable</t>
   </si>
   <si>
-    <t>verifyaddmedicine</t>
-  </si>
-  <si>
-    <t>crocin,Rohit,5</t>
-  </si>
-  <si>
-    <t>verifyaddmedicinewithotheroption</t>
-  </si>
-  <si>
-    <t>verifysearch_update_medicine</t>
-  </si>
-  <si>
-    <t>Abhishek,Rohit</t>
-  </si>
-  <si>
-    <t>verifysetreminder</t>
+    <t>t1_verifyaddmedicine</t>
+  </si>
+  <si>
+    <t>crocin,Rick,5</t>
+  </si>
+  <si>
+    <t>t2_verifyaddmedicinewithotheroption</t>
+  </si>
+  <si>
+    <t>t3_verifysearch_update_medicine</t>
+  </si>
+  <si>
+    <t>crocin,Vibhor,5</t>
+  </si>
+  <si>
+    <t>t4_verifysetreminder</t>
   </si>
   <si>
     <t>addvitalsigns</t>
@@ -255,22 +261,22 @@
     <t>vitalsigns_negativescenerios</t>
   </si>
   <si>
-    <t>addnote</t>
+    <t>t1_addnote</t>
   </si>
   <si>
     <t>vibhor954,Test Description,Updated Description</t>
   </si>
   <si>
-    <t>updatenote</t>
-  </si>
-  <si>
-    <t>verifysearch_note</t>
+    <t>t2_updatenote</t>
+  </si>
+  <si>
+    <t>t3_verifysearch_note</t>
   </si>
   <si>
     <t>vibhor954,Test Description</t>
   </si>
   <si>
-    <t>note_negativescenerios</t>
+    <t>t4_note_negativescenerios</t>
   </si>
   <si>
     <t>addphotofromgallery_cropimage</t>
@@ -361,9 +367,6 @@
   </si>
   <si>
     <t>addreminder</t>
-  </si>
-  <si>
-    <t>run</t>
   </si>
   <si>
     <t>Test_Reminder</t>
@@ -378,9 +381,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="28">
     <font>
@@ -436,6 +439,29 @@
       <sz val="10"/>
       <name val="Arial"/>
       <charset val="134"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <u/>
@@ -446,6 +472,88 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -461,78 +569,10 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -543,43 +583,6 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -590,55 +593,163 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -650,49 +761,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -704,73 +773,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -781,6 +784,30 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -840,6 +867,15 @@
     <border>
       <left/>
       <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top style="thin">
         <color theme="4"/>
       </top>
@@ -848,172 +884,139 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="3" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="7" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="8" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="4" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="9" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="8" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="7" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="8" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="8" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="8" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="8" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="8" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="27" fillId="31" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="8" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1382,7 +1385,7 @@
   <dimension ref="A1:B19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1015625" defaultRowHeight="14" outlineLevelCol="1"/>
@@ -1429,21 +1432,21 @@
       <c r="A5" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="5">
-        <v>10</v>
+      <c r="B5" s="5" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="6" ht="22" spans="1:2">
       <c r="A6" s="10" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="7" ht="22" spans="1:2">
       <c r="A7" s="10" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B7" s="5">
         <v>4723</v>
@@ -1451,15 +1454,15 @@
     </row>
     <row r="8" ht="22" spans="1:2">
       <c r="A8" s="10" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="9" ht="22" spans="1:2">
       <c r="A9" s="10" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B9" s="5">
         <v>13.3</v>
@@ -1467,39 +1470,39 @@
     </row>
     <row r="10" ht="22" spans="1:2">
       <c r="A10" s="10" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B10" s="5"/>
     </row>
     <row r="11" ht="22" spans="1:2">
       <c r="A11" s="10" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B11" s="12"/>
     </row>
     <row r="12" ht="22" spans="1:2">
       <c r="A12" s="10" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B12" s="5"/>
     </row>
     <row r="13" ht="22" spans="1:2">
       <c r="A13" s="10" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="14" ht="22" spans="1:2">
       <c r="A14" s="10" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B14" s="5"/>
     </row>
     <row r="15" ht="22" spans="1:2">
       <c r="A15" s="10" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B15" s="13" t="b">
         <f>FALSE()</f>
@@ -1508,34 +1511,34 @@
     </row>
     <row r="16" ht="22" spans="1:2">
       <c r="A16" s="10" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="17" ht="22" spans="1:2">
       <c r="A17" s="10" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="18" ht="22" spans="1:2">
       <c r="A18" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="B18" s="5" t="s">
         <v>26</v>
-      </c>
-      <c r="B18" s="5" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="19" ht="22" spans="1:2">
       <c r="A19" s="10" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -1559,7 +1562,7 @@
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5390625" defaultRowHeight="14" outlineLevelRow="5" outlineLevelCol="2"/>
@@ -1571,68 +1574,68 @@
   <sheetData>
     <row r="1" ht="22" spans="1:3">
       <c r="A1" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="2" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="2" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="2" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" t="s">
-        <v>72</v>
-      </c>
-      <c r="B5" t="s">
-        <v>32</v>
+        <v>74</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>33</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" t="s">
-        <v>73</v>
-      </c>
-      <c r="B6" t="s">
-        <v>32</v>
+        <v>75</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>33</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
     </row>
   </sheetData>
@@ -1651,7 +1654,7 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelRow="4" outlineLevelCol="2"/>
@@ -1663,57 +1666,57 @@
   <sheetData>
     <row r="1" ht="22" spans="1:3">
       <c r="A1" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="2" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C4" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="4" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C5" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
     </row>
   </sheetData>
@@ -1739,81 +1742,81 @@
   <sheetData>
     <row r="1" ht="22" spans="1:3">
       <c r="A1" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="2" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="4" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="4" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
     </row>
   </sheetData>
@@ -1839,57 +1842,57 @@
   <sheetData>
     <row r="1" ht="22" spans="1:3">
       <c r="A1" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="2" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="B3" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="B4" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="B5" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C5" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
     </row>
   </sheetData>
@@ -1916,46 +1919,46 @@
   <sheetData>
     <row r="1" ht="22" spans="1:3">
       <c r="A1" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="2" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="B3" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="B4" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
     </row>
   </sheetData>
@@ -1981,65 +1984,65 @@
   <sheetData>
     <row r="1" ht="22" spans="1:3">
       <c r="A1" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="2" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="B3" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="4" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="B4" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="B5" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="4" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="B6" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
     </row>
   </sheetData>
@@ -2064,30 +2067,30 @@
   <sheetData>
     <row r="1" ht="22" spans="1:3">
       <c r="A1" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="2" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C2" s="3"/>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="2" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="B3" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -2101,8 +2104,8 @@
   <sheetPr/>
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelRow="2" outlineLevelCol="2"/>
@@ -2113,32 +2116,32 @@
   <sheetData>
     <row r="1" ht="22" spans="1:3">
       <c r="A1" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="2" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>110</v>
+        <v>33</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="B3" t="s">
-        <v>110</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -2153,7 +2156,7 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.0703125" defaultRowHeight="14" outlineLevelRow="3" outlineLevelCol="2"/>
@@ -2165,39 +2168,39 @@
   <sheetData>
     <row r="1" ht="22" spans="1:3">
       <c r="A1" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="2" ht="22" spans="1:3">
       <c r="A2" s="5" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C2" s="8"/>
     </row>
     <row r="3" ht="22" spans="1:3">
       <c r="A3" s="5" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C3" s="8"/>
     </row>
     <row r="4" ht="22" spans="1:3">
       <c r="A4" s="5" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C4" s="8"/>
     </row>
@@ -2214,7 +2217,7 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.609375" defaultRowHeight="14" outlineLevelRow="2" outlineLevelCol="2"/>
@@ -2226,35 +2229,35 @@
   <sheetData>
     <row r="1" ht="22" spans="1:3">
       <c r="A1" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="2" ht="22" spans="1:3">
       <c r="A2" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>32</v>
+        <v>36</v>
+      </c>
+      <c r="B2" t="s">
+        <v>33</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B3" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>
@@ -2277,7 +2280,7 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.609375" defaultRowHeight="14" outlineLevelRow="2" outlineLevelCol="2"/>
@@ -2289,35 +2292,35 @@
   <sheetData>
     <row r="1" ht="22" spans="1:3">
       <c r="A1" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="2" ht="22" spans="1:3">
       <c r="A2" s="5" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="3" ht="22" spans="1:3">
       <c r="A3" s="5" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B3" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>
@@ -2337,7 +2340,7 @@
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.015625" defaultRowHeight="14" outlineLevelRow="6" outlineLevelCol="2"/>
@@ -2349,70 +2352,70 @@
   <sheetData>
     <row r="1" ht="22" spans="1:3">
       <c r="A1" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="2" ht="22" spans="1:3">
       <c r="A2" s="5" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>32</v>
+        <v>44</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
     </row>
     <row r="3" ht="22" spans="1:3">
       <c r="A3" s="4" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C3" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
     </row>
     <row r="4" ht="22" spans="1:2">
       <c r="A4" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="5" ht="22" spans="1:2">
       <c r="A5" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="6" ht="22" spans="1:2">
       <c r="A6" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="7" ht="22" spans="1:3">
       <c r="A7" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
     </row>
   </sheetData>
@@ -2432,7 +2435,7 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.015625" defaultRowHeight="14" outlineLevelRow="2" outlineLevelCol="2"/>
@@ -2444,30 +2447,30 @@
   <sheetData>
     <row r="1" ht="22" spans="1:3">
       <c r="A1" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="2" ht="22" spans="1:3">
       <c r="A2" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="B2" t="s">
-        <v>32</v>
+        <v>53</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>33</v>
       </c>
       <c r="C2" s="6"/>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" ht="22" spans="1:2">
       <c r="A3" t="s">
-        <v>52</v>
-      </c>
-      <c r="B3" t="s">
-        <v>32</v>
+        <v>54</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -2482,8 +2485,8 @@
   <sheetPr/>
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.015625" defaultRowHeight="14" outlineLevelRow="2" outlineLevelCol="2"/>
@@ -2494,30 +2497,30 @@
   <sheetData>
     <row r="1" ht="22" spans="1:3">
       <c r="A1" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="2" ht="22" spans="1:3">
       <c r="A2" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>32</v>
+        <v>55</v>
+      </c>
+      <c r="B2" t="s">
+        <v>33</v>
       </c>
       <c r="C2" s="6"/>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="B3" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -2533,7 +2536,7 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.015625" defaultRowHeight="14" outlineLevelRow="4" outlineLevelCol="2"/>
@@ -2545,57 +2548,57 @@
   <sheetData>
     <row r="1" ht="22" spans="1:3">
       <c r="A1" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="2" ht="22" spans="1:3">
-      <c r="A2" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B2" t="s">
+        <v>33</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="B3" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C3" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="B4" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C4" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="B5" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C5" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
     </row>
   </sheetData>
@@ -2608,13 +2611,13 @@
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.015625" defaultRowHeight="14" outlineLevelRow="5" outlineLevelCol="2"/>
+  <sheetFormatPr defaultColWidth="9.015625" defaultRowHeight="14" outlineLevelRow="4" outlineLevelCol="2"/>
   <cols>
     <col min="1" max="1" width="31.1171875" customWidth="1"/>
     <col min="2" max="2" width="27.46875" customWidth="1"/>
@@ -2623,68 +2626,57 @@
   <sheetData>
     <row r="1" ht="22" spans="1:3">
       <c r="A1" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="2" ht="22" spans="1:3">
-      <c r="A2" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" t="s">
+        <v>63</v>
+      </c>
+      <c r="B2" t="s">
+        <v>33</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="B3" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C3" t="s">
-        <v>58</v>
+        <v>64</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="B4" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>62</v>
+        <v>67</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" t="s">
-        <v>60</v>
+        <v>68</v>
       </c>
       <c r="B5" t="s">
-        <v>32</v>
-      </c>
-      <c r="C5" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
-      <c r="A6" t="s">
-        <v>66</v>
-      </c>
-      <c r="B6" t="s">
-        <v>32</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>62</v>
+        <v>33</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>67</v>
       </c>
     </row>
   </sheetData>

</xml_diff>